<commit_message>
Fix React routing, layout architecture and stabilize frontend
</commit_message>
<xml_diff>
--- a/Data/Study 1_Compiled_EDRR_updated.xlsx
+++ b/Data/Study 1_Compiled_EDRR_updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.novartis.net/personal/jagdasu3_novartis_net/Documents/Desktop/Anonymized Study Files/Study 1_CPID_Input Files - Anonymization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ClinIQ\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_8876721A72A2A1C8136FE6375AEA8CCADE140A30" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E3D2270-0A38-4705-8BFE-760B44DD4C37}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9561FF51-AFBE-4402-A6A5-4B64D1CE9C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="340" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenIssuesSummary" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -59,82 +57,82 @@
     <t>Subject 58</t>
   </si>
   <si>
+    <t>Subject 83</t>
+  </si>
+  <si>
+    <t>Subject 87</t>
+  </si>
+  <si>
+    <t>Subject 42</t>
+  </si>
+  <si>
+    <t>Subject 90</t>
+  </si>
+  <si>
+    <t>Subject 65</t>
+  </si>
+  <si>
+    <t>Subject 9</t>
+  </si>
+  <si>
+    <t>Subject 18</t>
+  </si>
+  <si>
+    <t>Subject 26</t>
+  </si>
+  <si>
+    <t>Subject 32</t>
+  </si>
+  <si>
+    <t>Subject 46</t>
+  </si>
+  <si>
+    <t>Subject 47</t>
+  </si>
+  <si>
+    <t>Subject 64</t>
+  </si>
+  <si>
+    <t>Subject 19</t>
+  </si>
+  <si>
+    <t>Subject 39</t>
+  </si>
+  <si>
+    <t>Subject 45</t>
+  </si>
+  <si>
+    <t>Subject 7</t>
+  </si>
+  <si>
+    <t>Subject 36</t>
+  </si>
+  <si>
+    <t>Subject 44</t>
+  </si>
+  <si>
+    <t>Subject 22</t>
+  </si>
+  <si>
+    <t>Subject 52</t>
+  </si>
+  <si>
+    <t>Subject 61</t>
+  </si>
+  <si>
+    <t>Subject 62</t>
+  </si>
+  <si>
+    <t>Subject 88</t>
+  </si>
+  <si>
+    <t>Subject 96</t>
+  </si>
+  <si>
+    <t>Subject 97</t>
+  </si>
+  <si>
     <t>Subject 78</t>
-  </si>
-  <si>
-    <t>Subject 83</t>
-  </si>
-  <si>
-    <t>Subject 87</t>
-  </si>
-  <si>
-    <t>Subject 42</t>
-  </si>
-  <si>
-    <t>Subject 90</t>
-  </si>
-  <si>
-    <t>Subject 65</t>
-  </si>
-  <si>
-    <t>Subject 9</t>
-  </si>
-  <si>
-    <t>Subject 18</t>
-  </si>
-  <si>
-    <t>Subject 26</t>
-  </si>
-  <si>
-    <t>Subject 32</t>
-  </si>
-  <si>
-    <t>Subject 46</t>
-  </si>
-  <si>
-    <t>Subject 47</t>
-  </si>
-  <si>
-    <t>Subject 64</t>
-  </si>
-  <si>
-    <t>Subject 19</t>
-  </si>
-  <si>
-    <t>Subject 39</t>
-  </si>
-  <si>
-    <t>Subject 45</t>
-  </si>
-  <si>
-    <t>Subject 7</t>
-  </si>
-  <si>
-    <t>Subject 36</t>
-  </si>
-  <si>
-    <t>Subject 44</t>
-  </si>
-  <si>
-    <t>Subject 22</t>
-  </si>
-  <si>
-    <t>Subject 52</t>
-  </si>
-  <si>
-    <t>Subject 61</t>
-  </si>
-  <si>
-    <t>Subject 62</t>
-  </si>
-  <si>
-    <t>Subject 88</t>
-  </si>
-  <si>
-    <t>Subject 96</t>
-  </si>
-  <si>
-    <t>Subject 97</t>
   </si>
 </sst>
 </file>
@@ -525,21 +523,21 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="3" customWidth="1"/>
     <col min="3" max="3" width="32" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -564,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -575,287 +573,287 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="C11" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C14" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C22" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
@@ -868,19 +866,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c2cee52-74d3-46f1-b334-c7f0d9663bb1">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c9ac3ab4-a7cc-4b3a-aeed-dd55a233ac4b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C2F4983DD335CF429A4CB33CFCACD7B4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d9baef14326416a0e8db21305cf9607">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7c2cee52-74d3-46f1-b334-c7f0d9663bb1" xmlns:ns3="3b1c506d-bf6f-415e-b438-4cee1daa8122" xmlns:ns4="c9ac3ab4-a7cc-4b3a-aeed-dd55a233ac4b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1a634a491c43f395dbfd0355a4d1c58" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1137,6 +1122,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7c2cee52-74d3-46f1-b334-c7f0d9663bb1">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c9ac3ab4-a7cc-4b3a-aeed-dd55a233ac4b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1147,18 +1145,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D77A67B-AF7F-4CDD-AB13-2B3AC34425AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="7c2cee52-74d3-46f1-b334-c7f0d9663bb1"/>
-    <ds:schemaRef ds:uri="c9ac3ab4-a7cc-4b3a-aeed-dd55a233ac4b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CD23B04-4142-4717-A933-1CA56FFA4190}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1179,6 +1165,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D77A67B-AF7F-4CDD-AB13-2B3AC34425AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="7c2cee52-74d3-46f1-b334-c7f0d9663bb1"/>
+    <ds:schemaRef ds:uri="c9ac3ab4-a7cc-4b3a-aeed-dd55a233ac4b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99EFC89B-711A-40AC-9CE2-9B32F061526E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Completed role-based auth, user portal, dashboard fixes
</commit_message>
<xml_diff>
--- a/Data/Study 1_Compiled_EDRR_updated.xlsx
+++ b/Data/Study 1_Compiled_EDRR_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ClinIQ\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9561FF51-AFBE-4402-A6A5-4B64D1CE9C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD73C8A-0522-4AEB-BCFC-3695B1FE2432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>